<commit_message>
Complete tool get new doc
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\kaito\coding\auto_update_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AA35B4-AB53-42C4-9231-E65D686D54EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1175E0-4631-4AF5-B95F-8B0EE208C609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="0" windowWidth="18135" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,28 @@
     <definedName name="dieu_3_1" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="tc_1" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Số TT</t>
   </si>
@@ -48,38 +59,14 @@
     <t>Nội dung giao cho địa phương</t>
   </si>
   <si>
-    <t>Quyết định</t>
-  </si>
-  <si>
-    <t>Số: 2229/QĐ-BTTTT ngày 19/12/2024 của Bộ Thông tin và Truyền thông</t>
-  </si>
-  <si>
-    <t>Quyết định ban hành khung tiêu chí, thành lập hội đồng và quy trình xác định thí điểm nền tảng số phục vụ người dân năm 2024, 2025</t>
-  </si>
-  <si>
-    <t>Không có</t>
-  </si>
-  <si>
-    <t>Thông tư</t>
-  </si>
-  <si>
-    <t>Đề nghị phòng BCVTCNTT rà soát và tham mưu</t>
-  </si>
-  <si>
-    <t>Thông tư ban hành “Quy chuẩn kỹ thuật quốc gia về thiết bị camera giám sát sử dụng giao thức Internet - Các yêu cầu an toàn thông tin cơ bản”</t>
-  </si>
-  <si>
     <t>Nội dung tham mưu HĐND, UBND tỉnh  cần ban hành mới, sửa đổi, bổ sung, thay thế; tiến độ thực hiện</t>
-  </si>
-  <si>
-    <t>Số: 21/2024/TT-BTTTT ngày xx/xx/xxxx của ….</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,12 +76,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -136,19 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,43 +435,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>